<commit_message>
Webdriver Listner & suite
</commit_message>
<xml_diff>
--- a/src/main/java/com/opencart/testdata/TestData.xlsx
+++ b/src/main/java/com/opencart/testdata/TestData.xlsx
@@ -40,16 +40,16 @@
     <t>Kush@123</t>
   </si>
   <si>
-    <t>Test12</t>
-  </si>
-  <si>
-    <t>Test124</t>
-  </si>
-  <si>
-    <t>kushaltest111@gmail.com</t>
-  </si>
-  <si>
-    <t>kushaltest221@gmail.com</t>
+    <t>Test1233</t>
+  </si>
+  <si>
+    <t>kushaltest11133@gmail.com</t>
+  </si>
+  <si>
+    <t>kushaltest22331@gmail.com</t>
+  </si>
+  <si>
+    <t>Test12455</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>8780921804</v>
@@ -472,10 +472,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>8700921864</v>

</xml_diff>